<commit_message>
correction of i2c register map
</commit_message>
<xml_diff>
--- a/docs/M5Stack_Step-Motor-Driver_V1_1_I2C.xlsx
+++ b/docs/M5Stack_Step-Motor-Driver_V1_1_I2C.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">M5STACK STEP MOTOR MODULE V1.1 I2C Protocol</t>
   </si>
@@ -57,27 +57,50 @@
     <t xml:space="preserve">note</t>
   </si>
   <si>
-    <t xml:space="preserve">Limit
-Input</t>
+    <t xml:space="preserve">/Limit/
+/Enable/
+/Fault/
+/Reset/</t>
   </si>
   <si>
     <t xml:space="preserve">0x00
-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit
-Byte0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read LSB 4 bits (nibbles or half byte) and each bit value is 0 or 1 depending on limit inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable
-Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x01
-W</t>
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Limit-
+Byte</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[1]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">R</t>
+    </r>
   </si>
   <si>
     <r>
@@ -98,56 +121,132 @@
         <family val="0"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">Byte0</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight-byte2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight-byte3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor enable = 0x00
-Motor disable = 0x10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fault
-Input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x04
-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fault-Byte0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read LSB 3 bits and each bit value is 0 or 1 depending on fault inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reset
-Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x05
-R/W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reset-Byte0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read/Write LSB 3 bits and each bit value is 0 or 1 </t>
+      <t xml:space="preserve">Byte</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[2]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">W</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Fault-Byte</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[3]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Reset-Byte</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[4]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">R/W</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Firmware Version</t>
   </si>
   <si>
-    <t xml:space="preserve">0xF0
-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
+    <t xml:space="preserve">0xFE
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Version
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">R</t>
+    </r>
   </si>
   <si>
     <r>
@@ -176,11 +275,32 @@
     <t xml:space="preserve">I2C Address</t>
   </si>
   <si>
-    <t xml:space="preserve">0xF0
-R/W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
+    <t xml:space="preserve">0xFF
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Address
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">R/W</t>
+    </r>
   </si>
   <si>
     <r>
@@ -203,6 +323,33 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> 1~127</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Read LSB 4 bits (nibbles or half byte) and each bit value is 0 or 1 depending on limit inputs
+2.Motor enable = 0x00
+   Motor disable = 0x10
+3.Read LSB 3 bits and each bit value is 0 or 1 depending on fault inputs
+4.Read/Write LSB 3 bits and each bit value is 0 or 1 </t>
     </r>
   </si>
 </sst>
@@ -269,14 +416,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑 Light"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑 Light"/>
@@ -291,7 +438,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,8 +463,14 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -381,6 +534,13 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="hair"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -407,7 +567,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,6 +612,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -460,22 +624,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -498,6 +646,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -512,7 +664,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -530,7 +682,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFDEADA"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFF2F2F2"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -577,10 +729,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:U1048576"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
+      <selection pane="topLeft" activeCell="S10" activeCellId="0" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -717,57 +869,57 @@
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="43" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="14" t="s">
+      <c r="T5" s="14"/>
+      <c r="U5" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -777,143 +929,70 @@
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="16" t="s">
+      <c r="U6" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+    <row r="7" customFormat="false" ht="93.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
     </row>
-    <row r="8" customFormat="false" ht="85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="17"/>
-      <c r="U8" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="U9" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="68" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="216.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="8">
     <mergeCell ref="A1:T2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="F4:T4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="F5:T5"/>
+    <mergeCell ref="E5:R5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="F6:T6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="F7:T7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:R8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:S9"/>
+    <mergeCell ref="E6:S6"/>
+    <mergeCell ref="A7:U7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>